<commit_message>
PCB basic design complete
basic design complete
</commit_message>
<xml_diff>
--- a/pcb/OECU_BASE/OECU_BASE_BOM.xlsx
+++ b/pcb/OECU_BASE/OECU_BASE_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.My_Tech_Studio\1.Project\MyOECU\pcb\OECU_BASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A9CDC90-310D-4E0E-B09A-B3880687973F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA843015-9E19-4190-954F-C1B44A77E982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30504" yWindow="0" windowWidth="23256" windowHeight="12576" xr2:uid="{E88DC1D3-7B2B-4C83-99BB-6B00AB105D89}"/>
+    <workbookView xWindow="30504" yWindow="0" windowWidth="23256" windowHeight="12576" xr2:uid="{4FC16DC2-95EA-477E-82E8-A2FED4D239D9}"/>
   </bookViews>
   <sheets>
     <sheet name="OECU_BASE_BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="135">
   <si>
     <t>Comment</t>
   </si>
@@ -86,9 +86,18 @@
     <t>47uF</t>
   </si>
   <si>
+    <t>贴片电容 1206</t>
+  </si>
+  <si>
     <t>C2, C3</t>
   </si>
   <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>CAP_1206</t>
+  </si>
+  <si>
     <t>22uF</t>
   </si>
   <si>
@@ -104,18 +113,9 @@
     <t>1nF 1KV</t>
   </si>
   <si>
-    <t>贴片电容 1206</t>
-  </si>
-  <si>
     <t>C57, C75, C93, C111, C129, C147</t>
   </si>
   <si>
-    <t>1206</t>
-  </si>
-  <si>
-    <t>CAP_1206</t>
-  </si>
-  <si>
     <t>DB25_1</t>
   </si>
   <si>
@@ -212,13 +212,13 @@
     <t>M1</t>
   </si>
   <si>
-    <t>MyJtag</t>
+    <t>MyJTAG</t>
   </si>
   <si>
     <t>M2</t>
   </si>
   <si>
-    <t>MYJATG_1</t>
+    <t>MyJatg_1</t>
   </si>
   <si>
     <t>MyJtag_1</t>
@@ -836,7 +836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B339671-9DD2-49E7-B764-3E12B043B938}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E0B8C7-CADF-41DC-B669-C55C7439B9FC}">
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -911,16 +911,16 @@
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1">
         <v>2</v>
@@ -928,19 +928,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
@@ -968,19 +968,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1">
         <v>6</v>
@@ -1150,7 +1150,9 @@
       <c r="A16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
@@ -1168,7 +1170,9 @@
       <c r="A17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
@@ -1186,7 +1190,9 @@
       <c r="A18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
@@ -1204,7 +1210,9 @@
       <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
@@ -1522,7 +1530,9 @@
       <c r="A35" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="1"/>
+      <c r="B35" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C35" s="2" t="s">
         <v>107</v>
       </c>
@@ -1600,7 +1610,9 @@
       <c r="A39" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C39" s="2" t="s">
         <v>120</v>
       </c>
@@ -1658,7 +1670,9 @@
       <c r="A42" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C42" s="2" t="s">
         <v>129</v>
       </c>

</xml_diff>